<commit_message>
feat: Add functionality to write year to Excel sheet and save workbook
- Implemented `writeYearToSheet(int year)` method in `ExcelExporter` to write the specified year to cell B7 in the Excel sheet.
- Updated `main.cpp` to call `writeYearToSheet` with the appropriate year before exporting statistics.
- Enhanced `saveWorkbook` method to ensure proper saving and releasing of the workbook.
- Added new test files and logs for better tracking of program execution and results.
- Updated version information to v1.0.0-9-g3ef9aa2.
- Removed outdated report files to maintain a clean report directory.
</commit_message>
<xml_diff>
--- a/cod_Migration/template/template_empty.xlsx
+++ b/cod_Migration/template/template_empty.xlsx
@@ -126,12 +126,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="0.00;[Red]0.00"/>
+    <numFmt numFmtId="176" formatCode="0.00_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="0.00_ "/>
+    <numFmt numFmtId="177" formatCode="0.00;[Red]0.00"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -151,16 +151,75 @@
     </font>
     <font>
       <b/>
-      <sz val="14"/>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -180,33 +239,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -226,6 +263,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -233,47 +271,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -287,16 +287,16 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -323,25 +323,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -353,157 +473,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -604,15 +604,103 @@
       <left style="medium">
         <color auto="1"/>
       </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
+      <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color auto="1"/>
       </left>
       <right style="thin">
@@ -623,100 +711,12 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color auto="1"/>
       </left>
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right/>
       <top/>
       <bottom/>
       <diagonal/>
@@ -1047,9 +1047,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
+      <left/>
       <right style="medium">
         <color auto="1"/>
       </right>
@@ -1071,7 +1069,9 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right style="medium">
         <color auto="1"/>
       </right>
@@ -1093,17 +1093,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1117,6 +1117,36 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -1141,32 +1171,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1179,168 +1190,157 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="53" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="54" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="52" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="54" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="53" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="49" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="50" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="47" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="47" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="49" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="52" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="50" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="50" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="51" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="48" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="48" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="48" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="51" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="48" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="47" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1365,75 +1365,81 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1503,28 +1509,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1605,8 +1611,8 @@
     <xf numFmtId="10" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
@@ -1614,49 +1620,52 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="3" borderId="1" xfId="47" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="3" borderId="2" xfId="47" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="2" xfId="47" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="3" borderId="1" xfId="47" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="3" borderId="2" xfId="47" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="2" xfId="47" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+    <xf numFmtId="10" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1990,7 +1999,7 @@
   <dimension ref="B1:K36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13:I16"/>
+      <selection activeCell="B6" sqref="B6:K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15"/>
@@ -2014,19 +2023,19 @@
       <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="41" t="s">
+      <c r="E2" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="62" t="s">
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="73" t="s">
+      <c r="J2" s="75" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="63" t="s">
+      <c r="K2" s="65" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2034,35 +2043,35 @@
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="44" t="s">
+      <c r="E3" s="46" t="s">
         <v>7</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="44" t="s">
+      <c r="G3" s="46" t="s">
         <v>9</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="64"/>
-      <c r="J3" s="74"/>
-      <c r="K3" s="65"/>
-    </row>
-    <row r="4" spans="2:11">
+      <c r="I3" s="66"/>
+      <c r="J3" s="76"/>
+      <c r="K3" s="67"/>
+    </row>
+    <row r="4" ht="15.75" spans="2:11">
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
-      <c r="E4" s="45"/>
+      <c r="E4" s="47"/>
       <c r="F4" s="3"/>
-      <c r="G4" s="45"/>
+      <c r="G4" s="47"/>
       <c r="H4" s="3"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="75"/>
-      <c r="K4" s="76"/>
-    </row>
-    <row r="5" spans="2:11">
+      <c r="I4" s="47"/>
+      <c r="J4" s="77"/>
+      <c r="K4" s="78"/>
+    </row>
+    <row r="5" ht="15.75" spans="2:11">
       <c r="B5" s="4" t="s">
         <v>11</v>
       </c>
@@ -2072,7 +2081,7 @@
       <c r="D5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="46" t="s">
+      <c r="E5" s="48" t="s">
         <v>13</v>
       </c>
       <c r="F5" s="6" t="s">
@@ -2081,19 +2090,17 @@
       <c r="G5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="47" t="s">
+      <c r="H5" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="77"/>
-      <c r="J5" s="78"/>
-      <c r="K5" s="77" t="s">
+      <c r="I5" s="79"/>
+      <c r="J5" s="80"/>
+      <c r="K5" s="79" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" ht="18.75" spans="2:11">
-      <c r="B6" s="7">
-        <v>2024</v>
-      </c>
+    <row r="6" ht="21" spans="2:11">
+      <c r="B6" s="7"/>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
@@ -2102,7 +2109,7 @@
       <c r="H6" s="8"/>
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
-      <c r="K6" s="79"/>
+      <c r="K6" s="81"/>
     </row>
     <row r="7" spans="2:11">
       <c r="B7" s="9" t="s">
@@ -2110,16 +2117,16 @@
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="11"/>
-      <c r="E7" s="48"/>
-      <c r="F7" s="49"/>
+      <c r="E7" s="50"/>
+      <c r="F7" s="51"/>
       <c r="G7" s="10"/>
-      <c r="H7" s="49"/>
-      <c r="I7" s="80"/>
-      <c r="J7" s="81" t="e">
+      <c r="H7" s="51"/>
+      <c r="I7" s="82"/>
+      <c r="J7" s="83" t="e">
         <f>I7/$I$19</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K7" s="82" t="s">
+      <c r="K7" s="84" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2127,16 +2134,16 @@
       <c r="B8" s="12"/>
       <c r="C8" s="13"/>
       <c r="D8" s="14"/>
-      <c r="E8" s="50"/>
-      <c r="F8" s="51"/>
+      <c r="E8" s="52"/>
+      <c r="F8" s="53"/>
       <c r="G8" s="13"/>
-      <c r="H8" s="51"/>
-      <c r="I8" s="83"/>
-      <c r="J8" s="84" t="e">
+      <c r="H8" s="53"/>
+      <c r="I8" s="85"/>
+      <c r="J8" s="86" t="e">
         <f>I8/$I$20</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K8" s="85" t="s">
+      <c r="K8" s="87" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2144,16 +2151,16 @@
       <c r="B9" s="12"/>
       <c r="C9" s="15"/>
       <c r="D9" s="16"/>
-      <c r="E9" s="52"/>
-      <c r="F9" s="53"/>
-      <c r="G9" s="54"/>
-      <c r="H9" s="55"/>
-      <c r="I9" s="86"/>
-      <c r="J9" s="87" t="e">
+      <c r="E9" s="54"/>
+      <c r="F9" s="55"/>
+      <c r="G9" s="56"/>
+      <c r="H9" s="57"/>
+      <c r="I9" s="88"/>
+      <c r="J9" s="89" t="e">
         <f>I9/$I$21</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K9" s="85" t="s">
+      <c r="K9" s="87" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2161,16 +2168,16 @@
       <c r="B10" s="12"/>
       <c r="C10" s="17"/>
       <c r="D10" s="16"/>
-      <c r="E10" s="52"/>
-      <c r="F10" s="53"/>
-      <c r="G10" s="54"/>
-      <c r="H10" s="55"/>
-      <c r="I10" s="86"/>
-      <c r="J10" s="87" t="e">
+      <c r="E10" s="54"/>
+      <c r="F10" s="55"/>
+      <c r="G10" s="56"/>
+      <c r="H10" s="57"/>
+      <c r="I10" s="88"/>
+      <c r="J10" s="89" t="e">
         <f>I10/$I$28</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K10" s="85" t="s">
+      <c r="K10" s="87" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2178,15 +2185,15 @@
       <c r="B11" s="18"/>
       <c r="C11" s="19"/>
       <c r="D11" s="20"/>
-      <c r="E11" s="56"/>
-      <c r="F11" s="57"/>
-      <c r="G11" s="58"/>
-      <c r="H11" s="59"/>
-      <c r="I11" s="88">
+      <c r="E11" s="58"/>
+      <c r="F11" s="59"/>
+      <c r="G11" s="60"/>
+      <c r="H11" s="61"/>
+      <c r="I11" s="90">
         <v>1</v>
       </c>
-      <c r="J11" s="89"/>
-      <c r="K11" s="90" t="s">
+      <c r="J11" s="91"/>
+      <c r="K11" s="92" t="s">
         <v>22</v>
       </c>
     </row>
@@ -2200,7 +2207,7 @@
       <c r="H12" s="22"/>
       <c r="I12" s="22"/>
       <c r="J12" s="22"/>
-      <c r="K12" s="91"/>
+      <c r="K12" s="93"/>
     </row>
     <row r="13" spans="2:11">
       <c r="B13" s="23" t="s">
@@ -2208,16 +2215,16 @@
       </c>
       <c r="C13" s="10"/>
       <c r="D13" s="11"/>
-      <c r="E13" s="48"/>
-      <c r="F13" s="49"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="49"/>
-      <c r="I13" s="80"/>
-      <c r="J13" s="81" t="e">
+      <c r="E13" s="10"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="50"/>
+      <c r="H13" s="51"/>
+      <c r="I13" s="82"/>
+      <c r="J13" s="83" t="e">
         <f>I13/$I$19</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K13" s="82" t="s">
+      <c r="K13" s="84" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2225,16 +2232,16 @@
       <c r="B14" s="24"/>
       <c r="C14" s="13"/>
       <c r="D14" s="14"/>
-      <c r="E14" s="50"/>
-      <c r="F14" s="51"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="51"/>
-      <c r="I14" s="83"/>
-      <c r="J14" s="84" t="e">
+      <c r="E14" s="13"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="52"/>
+      <c r="H14" s="53"/>
+      <c r="I14" s="85"/>
+      <c r="J14" s="86" t="e">
         <f>I14/$I$20</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K14" s="85" t="s">
+      <c r="K14" s="87" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2242,16 +2249,16 @@
       <c r="B15" s="24"/>
       <c r="C15" s="15"/>
       <c r="D15" s="16"/>
-      <c r="E15" s="52"/>
-      <c r="F15" s="53"/>
-      <c r="G15" s="52"/>
-      <c r="H15" s="53"/>
-      <c r="I15" s="86"/>
-      <c r="J15" s="87" t="e">
+      <c r="E15" s="17"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="54"/>
+      <c r="H15" s="55"/>
+      <c r="I15" s="88"/>
+      <c r="J15" s="89" t="e">
         <f>I15/$I$21</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K15" s="85" t="s">
+      <c r="K15" s="87" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2259,16 +2266,16 @@
       <c r="B16" s="24"/>
       <c r="C16" s="17"/>
       <c r="D16" s="16"/>
-      <c r="E16" s="52"/>
-      <c r="F16" s="53"/>
-      <c r="G16" s="52"/>
-      <c r="H16" s="53"/>
-      <c r="I16" s="92"/>
-      <c r="J16" s="87" t="e">
+      <c r="E16" s="17"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="54"/>
+      <c r="H16" s="55"/>
+      <c r="I16" s="94"/>
+      <c r="J16" s="89" t="e">
         <f>I16/$I$28</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K16" s="85" t="s">
+      <c r="K16" s="87" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2276,15 +2283,15 @@
       <c r="B17" s="25"/>
       <c r="C17" s="19"/>
       <c r="D17" s="20"/>
-      <c r="E17" s="56"/>
-      <c r="F17" s="57"/>
-      <c r="G17" s="56"/>
-      <c r="H17" s="57"/>
-      <c r="I17" s="88">
+      <c r="E17" s="19"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="58"/>
+      <c r="H17" s="59"/>
+      <c r="I17" s="90">
         <v>1</v>
       </c>
-      <c r="J17" s="89"/>
-      <c r="K17" s="90" t="s">
+      <c r="J17" s="91"/>
+      <c r="K17" s="92" t="s">
         <v>22</v>
       </c>
     </row>
@@ -2298,190 +2305,190 @@
       <c r="H18" s="22"/>
       <c r="I18" s="22"/>
       <c r="J18" s="22"/>
-      <c r="K18" s="91"/>
+      <c r="K18" s="93"/>
     </row>
     <row r="19" spans="2:11">
       <c r="B19" s="26" t="s">
         <v>25</v>
       </c>
       <c r="C19" s="10">
-        <f>C7+C13</f>
+        <f t="shared" ref="C19:I19" si="0">C7+C13</f>
         <v>0</v>
       </c>
       <c r="D19" s="11">
-        <f>D7+D13</f>
-        <v>0</v>
-      </c>
-      <c r="E19" s="48">
-        <f>E7+E13</f>
-        <v>0</v>
-      </c>
-      <c r="F19" s="49">
-        <f>F7+F13</f>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E19" s="50">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F19" s="51">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G19" s="10">
-        <f>G7+G13</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H19" s="11">
-        <f>H7+H13</f>
-        <v>0</v>
-      </c>
-      <c r="I19" s="93">
-        <f>I7+I13</f>
-        <v>0</v>
-      </c>
-      <c r="J19" s="94">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I19" s="95">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J19" s="96">
         <v>1</v>
       </c>
-      <c r="K19" s="95" t="s">
+      <c r="K19" s="97" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="20" spans="2:11">
       <c r="B20" s="27"/>
       <c r="C20" s="13">
-        <f>C8+C14</f>
+        <f t="shared" ref="C20:I20" si="1">C8+C14</f>
         <v>0</v>
       </c>
       <c r="D20" s="14">
-        <f>D8+D14</f>
-        <v>0</v>
-      </c>
-      <c r="E20" s="50">
-        <f>E8+E14</f>
-        <v>0</v>
-      </c>
-      <c r="F20" s="51">
-        <f>F8+F14</f>
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E20" s="52">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F20" s="53">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G20" s="13">
-        <f>G8+G14</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H20" s="14">
-        <f>H8+H14</f>
-        <v>0</v>
-      </c>
-      <c r="I20" s="96">
-        <f>I8+I14</f>
-        <v>0</v>
-      </c>
-      <c r="J20" s="97">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I20" s="98">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J20" s="99">
         <v>1</v>
       </c>
-      <c r="K20" s="98" t="s">
+      <c r="K20" s="100" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="21" spans="2:11">
       <c r="B21" s="27"/>
       <c r="C21" s="15">
-        <f>C9+C15</f>
+        <f t="shared" ref="C21:H21" si="2">C9+C15</f>
         <v>0</v>
       </c>
       <c r="D21" s="16">
-        <f>D9+D15</f>
-        <v>0</v>
-      </c>
-      <c r="E21" s="52">
-        <f>E9+E15</f>
-        <v>0</v>
-      </c>
-      <c r="F21" s="53">
-        <f>F9+F15</f>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E21" s="54">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F21" s="55">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G21" s="17">
-        <f>G9+G15</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H21" s="16">
-        <f>H9+H15</f>
-        <v>0</v>
-      </c>
-      <c r="I21" s="99">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I21" s="101">
         <f>SUM(C21:H21)</f>
         <v>0</v>
       </c>
-      <c r="J21" s="100">
+      <c r="J21" s="102">
         <v>1</v>
       </c>
-      <c r="K21" s="98" t="s">
+      <c r="K21" s="100" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="22" spans="2:11">
       <c r="B22" s="27"/>
       <c r="C22" s="17" t="e">
-        <f>C21/C20</f>
+        <f t="shared" ref="C22:H22" si="3">C21/C20</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D22" s="16" t="e">
-        <f>D21/D20</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E22" s="52" t="e">
-        <f>E21/E20</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F22" s="53" t="e">
-        <f>F21/F20</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G22" s="60" t="e">
-        <f>G21/G20</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H22" s="61" t="e">
-        <f>H21/H20</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I22" s="101" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E22" s="54" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F22" s="55" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G22" s="62" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H22" s="63" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I22" s="103" t="e">
         <f>AVERAGE(C22:H22)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J22" s="87" t="e">
+      <c r="J22" s="89" t="e">
         <f>I22/I28</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K22" s="98" t="s">
+      <c r="K22" s="100" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="23" ht="15.75" spans="2:11">
       <c r="B23" s="28"/>
       <c r="C23" s="19" t="e">
-        <f>C21/$I$21</f>
+        <f t="shared" ref="C23:H23" si="4">C21/$I$21</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D23" s="20" t="e">
-        <f>D21/$I$21</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E23" s="56" t="e">
-        <f>E21/$I$21</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F23" s="57" t="e">
-        <f>F21/$I$21</f>
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E23" s="58" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F23" s="59" t="e">
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="G23" s="19" t="e">
-        <f>G21/$I$21</f>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H23" s="20" t="e">
-        <f>H21/$I$21</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I23" s="102">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I23" s="104">
         <v>1</v>
       </c>
-      <c r="J23" s="89"/>
-      <c r="K23" s="103" t="s">
+      <c r="J23" s="91"/>
+      <c r="K23" s="105" t="s">
         <v>22</v>
       </c>
     </row>
@@ -2495,7 +2502,7 @@
       <c r="H24" s="30"/>
       <c r="I24" s="30"/>
       <c r="J24" s="30"/>
-      <c r="K24" s="104"/>
+      <c r="K24" s="106"/>
     </row>
     <row r="25" spans="2:11">
       <c r="B25" s="9" t="s">
@@ -2509,22 +2516,22 @@
         <f>D13</f>
         <v>0</v>
       </c>
-      <c r="E25" s="62">
+      <c r="E25" s="64">
         <f>SUM(E19:H19)</f>
         <v>0</v>
       </c>
-      <c r="F25" s="62"/>
-      <c r="G25" s="62"/>
-      <c r="H25" s="63"/>
-      <c r="I25" s="93">
+      <c r="F25" s="64"/>
+      <c r="G25" s="64"/>
+      <c r="H25" s="65"/>
+      <c r="I25" s="95">
         <f>SUM(C25:H25)</f>
         <v>0</v>
       </c>
-      <c r="J25" s="105" t="e">
+      <c r="J25" s="107" t="e">
         <f>I25/I19</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K25" s="95" t="s">
+      <c r="K25" s="97" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2536,22 +2543,22 @@
       <c r="D26" s="14">
         <v>175</v>
       </c>
-      <c r="E26" s="64">
+      <c r="E26" s="66">
         <f>SUM(E20:H20)</f>
         <v>0</v>
       </c>
-      <c r="F26" s="64"/>
-      <c r="G26" s="64"/>
-      <c r="H26" s="65"/>
-      <c r="I26" s="96">
+      <c r="F26" s="66"/>
+      <c r="G26" s="66"/>
+      <c r="H26" s="67"/>
+      <c r="I26" s="98">
         <f>SUM(C26:H26)</f>
         <v>204</v>
       </c>
-      <c r="J26" s="84" t="e">
+      <c r="J26" s="86" t="e">
         <f>I26/I20</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K26" s="98" t="s">
+      <c r="K26" s="100" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2565,22 +2572,22 @@
         <f>D15</f>
         <v>0</v>
       </c>
-      <c r="E27" s="66">
+      <c r="E27" s="68">
         <f>SUM(E21:H21)</f>
         <v>0</v>
       </c>
-      <c r="F27" s="66"/>
-      <c r="G27" s="66"/>
-      <c r="H27" s="67"/>
-      <c r="I27" s="99">
+      <c r="F27" s="68"/>
+      <c r="G27" s="68"/>
+      <c r="H27" s="69"/>
+      <c r="I27" s="101">
         <f>SUM(C27:H27)</f>
         <v>0</v>
       </c>
-      <c r="J27" s="87" t="e">
+      <c r="J27" s="89" t="e">
         <f>I27/I21</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K27" s="98" t="s">
+      <c r="K27" s="100" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2594,195 +2601,195 @@
         <f>D16</f>
         <v>0</v>
       </c>
-      <c r="E28" s="66" t="e">
+      <c r="E28" s="68" t="e">
         <f>E27/E26</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F28" s="66"/>
-      <c r="G28" s="66"/>
-      <c r="H28" s="67"/>
-      <c r="I28" s="101" t="e">
+      <c r="F28" s="68"/>
+      <c r="G28" s="68"/>
+      <c r="H28" s="69"/>
+      <c r="I28" s="103" t="e">
         <f>AVERAGE(C28:H28)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J28" s="100">
+      <c r="J28" s="102">
         <v>1</v>
       </c>
-      <c r="K28" s="98" t="s">
+      <c r="K28" s="100" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="29" ht="15.75" spans="2:11">
       <c r="B29" s="18"/>
-      <c r="C29" s="19" t="e">
+      <c r="C29" s="31" t="e">
         <f>C27/I27</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D29" s="20" t="e">
+      <c r="D29" s="32" t="e">
         <f>D27/I27</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E29" s="68" t="e">
+      <c r="E29" s="70" t="e">
         <f>E27/I27</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F29" s="69"/>
-      <c r="G29" s="69"/>
-      <c r="H29" s="70"/>
-      <c r="I29" s="102">
+      <c r="F29" s="71"/>
+      <c r="G29" s="71"/>
+      <c r="H29" s="72"/>
+      <c r="I29" s="108">
         <v>1</v>
       </c>
-      <c r="J29" s="89"/>
-      <c r="K29" s="103" t="s">
+      <c r="J29" s="91"/>
+      <c r="K29" s="105" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="30" ht="15.75"/>
     <row r="31" spans="2:11">
-      <c r="B31" s="31" t="s">
+      <c r="B31" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="C31" s="31" t="s">
+      <c r="C31" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="D31" s="32"/>
-      <c r="E31" s="71" t="s">
+      <c r="D31" s="34"/>
+      <c r="E31" s="73" t="s">
         <v>29</v>
       </c>
-      <c r="F31" s="71"/>
-      <c r="G31" s="31" t="s">
+      <c r="F31" s="73"/>
+      <c r="G31" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="H31" s="32"/>
-      <c r="I31" s="71" t="s">
+      <c r="H31" s="34"/>
+      <c r="I31" s="73" t="s">
         <v>31</v>
       </c>
-      <c r="J31" s="71"/>
-      <c r="K31" s="106" t="s">
+      <c r="J31" s="73"/>
+      <c r="K31" s="109" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="2:11">
-      <c r="B32" s="33"/>
-      <c r="C32" s="33"/>
-      <c r="D32" s="34"/>
-      <c r="E32" s="72"/>
-      <c r="F32" s="72"/>
-      <c r="G32" s="33"/>
-      <c r="H32" s="34"/>
-      <c r="I32" s="72"/>
-      <c r="J32" s="72"/>
-      <c r="K32" s="107"/>
+    <row r="32" ht="15.75" spans="2:11">
+      <c r="B32" s="35"/>
+      <c r="C32" s="35"/>
+      <c r="D32" s="36"/>
+      <c r="E32" s="74"/>
+      <c r="F32" s="74"/>
+      <c r="G32" s="35"/>
+      <c r="H32" s="36"/>
+      <c r="I32" s="74"/>
+      <c r="J32" s="74"/>
+      <c r="K32" s="110"/>
     </row>
     <row r="33" ht="18" customHeight="1" spans="2:11">
-      <c r="B33" s="35" t="s">
+      <c r="B33" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="C33" s="36">
+      <c r="C33" s="38">
         <f>C7+D7</f>
         <v>0</v>
       </c>
-      <c r="D33" s="37"/>
-      <c r="E33" s="36">
+      <c r="D33" s="39"/>
+      <c r="E33" s="38">
         <f>C13</f>
         <v>0</v>
       </c>
-      <c r="F33" s="37"/>
-      <c r="G33" s="36">
+      <c r="F33" s="39"/>
+      <c r="G33" s="38">
         <f>D13</f>
         <v>0</v>
       </c>
-      <c r="H33" s="37"/>
-      <c r="I33" s="36">
+      <c r="H33" s="39"/>
+      <c r="I33" s="38">
         <f>E25</f>
         <v>0</v>
       </c>
-      <c r="J33" s="37"/>
-      <c r="K33" s="37">
+      <c r="J33" s="39"/>
+      <c r="K33" s="39">
         <v>970</v>
       </c>
     </row>
     <row r="34" ht="18" customHeight="1" spans="2:11">
-      <c r="B34" s="38" t="s">
+      <c r="B34" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="C34" s="39">
+      <c r="C34" s="41">
         <f>C33/$K$33</f>
         <v>0</v>
       </c>
-      <c r="D34" s="40"/>
-      <c r="E34" s="39">
+      <c r="D34" s="42"/>
+      <c r="E34" s="41">
         <f>E33/$K$33</f>
         <v>0</v>
       </c>
-      <c r="F34" s="40"/>
-      <c r="G34" s="39">
+      <c r="F34" s="42"/>
+      <c r="G34" s="41">
         <f>G33/$K$33</f>
         <v>0</v>
       </c>
-      <c r="H34" s="40"/>
-      <c r="I34" s="39">
+      <c r="H34" s="42"/>
+      <c r="I34" s="41">
         <f>I33/$K$33</f>
         <v>0</v>
       </c>
-      <c r="J34" s="40"/>
-      <c r="K34" s="108">
+      <c r="J34" s="42"/>
+      <c r="K34" s="111">
         <v>1</v>
       </c>
     </row>
     <row r="35" ht="18" customHeight="1" spans="2:11">
-      <c r="B35" s="35" t="s">
+      <c r="B35" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="C35" s="36">
+      <c r="C35" s="38">
         <f>C9+D9</f>
         <v>0</v>
       </c>
-      <c r="D35" s="37"/>
-      <c r="E35" s="36">
+      <c r="D35" s="39"/>
+      <c r="E35" s="38">
         <f>C15</f>
         <v>0</v>
       </c>
-      <c r="F35" s="37"/>
-      <c r="G35" s="36">
+      <c r="F35" s="39"/>
+      <c r="G35" s="38">
         <f>D15</f>
         <v>0</v>
       </c>
-      <c r="H35" s="37"/>
-      <c r="I35" s="36">
+      <c r="H35" s="39"/>
+      <c r="I35" s="38">
         <f>E27</f>
         <v>0</v>
       </c>
-      <c r="J35" s="37"/>
-      <c r="K35" s="37">
+      <c r="J35" s="39"/>
+      <c r="K35" s="39">
         <v>770205154.8</v>
       </c>
     </row>
     <row r="36" ht="18" customHeight="1" spans="2:11">
-      <c r="B36" s="38" t="s">
+      <c r="B36" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="C36" s="39">
+      <c r="C36" s="41">
         <f>C35/$K$35</f>
         <v>0</v>
       </c>
-      <c r="D36" s="40"/>
-      <c r="E36" s="39">
+      <c r="D36" s="42"/>
+      <c r="E36" s="41">
         <f>E35/$K$35</f>
         <v>0</v>
       </c>
-      <c r="F36" s="40"/>
-      <c r="G36" s="39">
+      <c r="F36" s="42"/>
+      <c r="G36" s="41">
         <f>G35/$K$35</f>
         <v>0</v>
       </c>
-      <c r="H36" s="40"/>
-      <c r="I36" s="39">
+      <c r="H36" s="42"/>
+      <c r="I36" s="41">
         <f>I35/$K$35</f>
         <v>0</v>
       </c>
-      <c r="J36" s="40"/>
-      <c r="K36" s="108">
+      <c r="J36" s="42"/>
+      <c r="K36" s="111">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update import script and add new log and report files
- Changed the CSV file path in import_client_activity.sh to use client_activity_1.csv.
- Added a new log file for the program execution on 2025-06-20, capturing various statistics and export success messages.
- Created multiple new Excel report files for different time stamps on 2025-06-20, documenting the exported statistics.
- Added two new reports with non-ASCII characters in their filenames.
- Updated the template_empty.xlsx file with new content.
</commit_message>
<xml_diff>
--- a/cod_Migration/template/template_empty.xlsx
+++ b/cod_Migration/template/template_empty.xlsx
@@ -4,12 +4,25 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27810" windowHeight="12375"/>
+    <workbookView windowWidth="28800" windowHeight="12465"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -124,14 +137,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="0.00_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="0.00;[Red]0.00"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="0.00;[Red]0.00"/>
+    <numFmt numFmtId="179" formatCode="0.00_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -158,82 +171,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -247,40 +187,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -295,12 +219,101 @@
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -323,37 +336,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -365,145 +510,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1093,17 +1106,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1117,36 +1130,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -1157,27 +1140,46 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1190,153 +1192,164 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="54" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="53" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="49" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="52" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="50" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="50" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="51" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="48" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="47" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="48" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="48" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="49" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="48" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="47" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="50" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="51" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="50" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="52" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="53" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="54" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1386,7 +1399,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1">
@@ -1590,7 +1603,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="1" fillId="3" borderId="1" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="10" fontId="1" fillId="3" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1">
@@ -1623,13 +1636,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+    <xf numFmtId="179" fontId="1" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="3" borderId="1" xfId="47" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="9" fontId="1" fillId="3" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1">
@@ -1638,7 +1651,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="3" borderId="2" xfId="47" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="9" fontId="1" fillId="3" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
@@ -1647,10 +1660,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="2" xfId="47" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="1" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1680,54 +1693,54 @@
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
-    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
-    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
-    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
-    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
-    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
-    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
-    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
-    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
-    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
-    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
-    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
-    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
-    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
-    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
-    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
     <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
-    <cellStyle name="Total" xfId="25" builtinId="25"/>
-    <cellStyle name="Output" xfId="26" builtinId="21"/>
-    <cellStyle name="Currency" xfId="27" builtinId="4"/>
-    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
-    <cellStyle name="Note" xfId="29" builtinId="10"/>
-    <cellStyle name="Input" xfId="30" builtinId="20"/>
-    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
-    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
-    <cellStyle name="Good" xfId="33" builtinId="26"/>
-    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
-    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
-    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
-    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
-    <cellStyle name="Title" xfId="39" builtinId="15"/>
-    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
-    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
-    <cellStyle name="Comma" xfId="44" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
-    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
-    <cellStyle name="Percent" xfId="47" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1999,7 +2012,7 @@
   <dimension ref="B1:K36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:K6"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15"/>
@@ -2538,10 +2551,10 @@
     <row r="26" spans="2:11">
       <c r="B26" s="12"/>
       <c r="C26" s="13">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="D26" s="14">
-        <v>175</v>
+        <v>0</v>
       </c>
       <c r="E26" s="66">
         <f>SUM(E20:H20)</f>
@@ -2552,7 +2565,7 @@
       <c r="H26" s="67"/>
       <c r="I26" s="98">
         <f>SUM(C26:H26)</f>
-        <v>204</v>
+        <v>0</v>
       </c>
       <c r="J26" s="86" t="e">
         <f>I26/I20</f>
@@ -2669,7 +2682,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="32" ht="15.75" spans="2:11">
+    <row r="32" spans="2:11">
       <c r="B32" s="35"/>
       <c r="C32" s="35"/>
       <c r="D32" s="36"/>
@@ -2706,31 +2719,32 @@
       </c>
       <c r="J33" s="39"/>
       <c r="K33" s="39">
-        <v>970</v>
+        <f>C33+E33+G33+I33</f>
+        <v>0</v>
       </c>
     </row>
     <row r="34" ht="18" customHeight="1" spans="2:11">
       <c r="B34" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="C34" s="41">
+      <c r="C34" s="41" t="e">
         <f>C33/$K$33</f>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="D34" s="42"/>
-      <c r="E34" s="41">
+      <c r="E34" s="41" t="e">
         <f>E33/$K$33</f>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="F34" s="42"/>
-      <c r="G34" s="41">
+      <c r="G34" s="41" t="e">
         <f>G33/$K$33</f>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="H34" s="42"/>
-      <c r="I34" s="41">
+      <c r="I34" s="41" t="e">
         <f>I33/$K$33</f>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="J34" s="42"/>
       <c r="K34" s="111">
@@ -2762,31 +2776,32 @@
       </c>
       <c r="J35" s="39"/>
       <c r="K35" s="39">
-        <v>770205154.8</v>
+        <f>C35+E35+G35+I35</f>
+        <v>0</v>
       </c>
     </row>
     <row r="36" ht="18" customHeight="1" spans="2:11">
       <c r="B36" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="C36" s="41">
+      <c r="C36" s="41" t="e">
         <f>C35/$K$35</f>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="D36" s="42"/>
-      <c r="E36" s="41">
+      <c r="E36" s="41" t="e">
         <f>E35/$K$35</f>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="F36" s="42"/>
-      <c r="G36" s="41">
+      <c r="G36" s="41" t="e">
         <f>G35/$K$35</f>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="H36" s="42"/>
-      <c r="I36" s="41">
+      <c r="I36" s="41" t="e">
         <f>I35/$K$35</f>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="J36" s="42"/>
       <c r="K36" s="111">

</xml_diff>

<commit_message>
feat(migration): update import scripts and logging
- Added a new image file `bd_shema_19.06.25.jpeg` to the migration documentation.
- Modified `import_client_activity.sh` to remove `client_activity_id` from the temporary table and update the main table with new or modified records. Added logging for the number of records added/updated.
- Updated `import_client_units.sh` to change the CSV file source and added logging for the number of records in the temporary table, existing records, and added records.
- Deleted the old log file `import_log.txt`.
- Added new Excel files for migration data.
- Updated `debug.sh` to comment out the debug ID line.
- Created new log files for program execution on various dates, capturing connection status and export success.
- Added new statistics report Excel files for the specified dates.
- Updated template file `template_empty.xlsx`.
</commit_message>
<xml_diff>
--- a/cod_Migration/template/template_empty.xlsx
+++ b/cod_Migration/template/template_empty.xlsx
@@ -2012,7 +2012,7 @@
   <dimension ref="B1:K36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L31" sqref="L31"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15"/>
@@ -2551,9 +2551,11 @@
     <row r="26" spans="2:11">
       <c r="B26" s="12"/>
       <c r="C26" s="13">
+        <f>C14</f>
         <v>0</v>
       </c>
       <c r="D26" s="14">
+        <f>D14</f>
         <v>0</v>
       </c>
       <c r="E26" s="66">

</xml_diff>